<commit_message>
test RFECV plot yb
</commit_message>
<xml_diff>
--- a/Input_data/NPs/NP_Database2.xlsx
+++ b/Input_data/NPs/NP_Database2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmp95\PycharmProjects\PC_ML_using NetSurfP\Input_data\NPs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pouls\PycharmProjects\PC_ML_using_NSP\Input_data\NPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4919658F-2B15-465F-9E63-F097EA2F333C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6935F2F1-DA42-4E35-903F-918C1E5176BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
+    <workbookView xWindow="855" yWindow="1170" windowWidth="27945" windowHeight="11385" activeTab="1" xr2:uid="{1E6018AB-3209-43BE-913D-2054D4E06304}"/>
   </bookViews>
   <sheets>
     <sheet name="NPUNID" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="119">
   <si>
     <t>NPID</t>
   </si>
@@ -369,6 +369,30 @@
   </si>
   <si>
     <t>ProteinID</t>
+  </si>
+  <si>
+    <t>P25_HS_100</t>
+  </si>
+  <si>
+    <t>Large_Citrate_HS_100</t>
+  </si>
+  <si>
+    <t>c200_HS_100</t>
+  </si>
+  <si>
+    <t>Small_Citrate_HS_100</t>
+  </si>
+  <si>
+    <t>PS_PEG_100</t>
+  </si>
+  <si>
+    <t>PS_Carb_HS_10</t>
+  </si>
+  <si>
+    <t>PS_Carb_HS_100</t>
+  </si>
+  <si>
+    <t>HS</t>
   </si>
 </sst>
 </file>
@@ -420,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -489,12 +513,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -533,6 +577,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,8 +656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E048F05F-71E8-4C64-93E3-98D61C308956}" name="Table1" displayName="Table1" ref="A1:Y37" totalsRowShown="0">
-  <autoFilter ref="A1:Y37" xr:uid="{E048F05F-71E8-4C64-93E3-98D61C308956}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E048F05F-71E8-4C64-93E3-98D61C308956}" name="Table1" displayName="Table1" ref="A1:Y44" totalsRowShown="0">
+  <autoFilter ref="A1:Y44" xr:uid="{E048F05F-71E8-4C64-93E3-98D61C308956}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y29">
     <sortCondition ref="A1:A29"/>
   </sortState>
@@ -946,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD93B0A-7305-43B0-9C03-61303B4AF43A}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,6 +2037,149 @@
         <v>65136</v>
       </c>
     </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>37</v>
+      </c>
+      <c r="C52">
+        <v>86</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="20">
+        <v>7</v>
+      </c>
+      <c r="F52" s="22">
+        <v>102843</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>38</v>
+      </c>
+      <c r="C53">
+        <v>87</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="20">
+        <v>7</v>
+      </c>
+      <c r="F53" s="14">
+        <v>102844</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>39</v>
+      </c>
+      <c r="C54">
+        <v>88</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="20">
+        <v>7</v>
+      </c>
+      <c r="F54" s="22">
+        <v>102845</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>40</v>
+      </c>
+      <c r="C55">
+        <v>89</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="20">
+        <v>7</v>
+      </c>
+      <c r="F55" s="14">
+        <v>102846</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>41</v>
+      </c>
+      <c r="C56">
+        <v>90</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" s="20">
+        <v>7</v>
+      </c>
+      <c r="F56" s="22">
+        <v>102847</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>42</v>
+      </c>
+      <c r="C57">
+        <v>91</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" s="20">
+        <v>7</v>
+      </c>
+      <c r="F57" s="14">
+        <v>102848</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>43</v>
+      </c>
+      <c r="C58">
+        <v>92</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" s="20">
+        <v>7</v>
+      </c>
+      <c r="F58" s="22">
+        <v>102849</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1985,16 +2187,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FB506C-18F9-4EF7-A2FE-9BAF44A578A1}">
-  <dimension ref="A1:Y37"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="19.140625" customWidth="1"/>
@@ -2007,6 +2209,7 @@
     <col min="21" max="21" width="34.5703125" customWidth="1"/>
     <col min="22" max="22" width="28.5703125" customWidth="1"/>
     <col min="23" max="23" width="26.28515625" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2901,7 +3104,7 @@
       <c r="M11" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11">
         <v>200</v>
       </c>
       <c r="O11">
@@ -2986,7 +3189,7 @@
       <c r="M12" t="s">
         <v>56</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12">
         <v>200</v>
       </c>
       <c r="O12">
@@ -4346,7 +4549,7 @@
       <c r="M28" t="s">
         <v>96</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N28">
         <v>200</v>
       </c>
       <c r="O28">
@@ -5146,6 +5349,601 @@
       </c>
       <c r="Y37" s="18" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>-21</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M38" t="s">
+        <v>24</v>
+      </c>
+      <c r="N38">
+        <v>378</v>
+      </c>
+      <c r="O38">
+        <v>410</v>
+      </c>
+      <c r="P38">
+        <v>410</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <v>3</v>
+      </c>
+      <c r="T38" t="s">
+        <v>118</v>
+      </c>
+      <c r="U38">
+        <v>5</v>
+      </c>
+      <c r="V38">
+        <v>44.6</v>
+      </c>
+      <c r="W38">
+        <v>30</v>
+      </c>
+      <c r="X38">
+        <v>25</v>
+      </c>
+      <c r="Y38" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>-49</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>57</v>
+      </c>
+      <c r="N39">
+        <v>182</v>
+      </c>
+      <c r="O39">
+        <v>229</v>
+      </c>
+      <c r="P39">
+        <v>229</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+      <c r="T39" t="s">
+        <v>118</v>
+      </c>
+      <c r="U39">
+        <v>10</v>
+      </c>
+      <c r="V39">
+        <v>44.6</v>
+      </c>
+      <c r="W39">
+        <v>30</v>
+      </c>
+      <c r="X39">
+        <v>25</v>
+      </c>
+      <c r="Y39" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>-38</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>56</v>
+      </c>
+      <c r="N40">
+        <v>100</v>
+      </c>
+      <c r="O40">
+        <v>230</v>
+      </c>
+      <c r="P40">
+        <v>230</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>3</v>
+      </c>
+      <c r="T40" t="s">
+        <v>118</v>
+      </c>
+      <c r="U40">
+        <v>5</v>
+      </c>
+      <c r="V40">
+        <v>44.6</v>
+      </c>
+      <c r="W40">
+        <v>30</v>
+      </c>
+      <c r="X40">
+        <v>25</v>
+      </c>
+      <c r="Y40" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>-42</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>57</v>
+      </c>
+      <c r="N41">
+        <v>82</v>
+      </c>
+      <c r="O41" s="4">
+        <v>149</v>
+      </c>
+      <c r="P41" s="4">
+        <v>149</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>3</v>
+      </c>
+      <c r="T41" t="s">
+        <v>118</v>
+      </c>
+      <c r="U41">
+        <v>10</v>
+      </c>
+      <c r="V41">
+        <v>44.6</v>
+      </c>
+      <c r="W41">
+        <v>30</v>
+      </c>
+      <c r="X41">
+        <v>25</v>
+      </c>
+      <c r="Y41" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>-7</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M42" t="s">
+        <v>96</v>
+      </c>
+      <c r="N42">
+        <v>200</v>
+      </c>
+      <c r="O42">
+        <v>221</v>
+      </c>
+      <c r="P42">
+        <v>266</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <v>3</v>
+      </c>
+      <c r="T42" t="s">
+        <v>118</v>
+      </c>
+      <c r="U42">
+        <v>1.6</v>
+      </c>
+      <c r="V42">
+        <v>44.6</v>
+      </c>
+      <c r="W42">
+        <v>30</v>
+      </c>
+      <c r="X42">
+        <v>25</v>
+      </c>
+      <c r="Y42" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>-63</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>56</v>
+      </c>
+      <c r="N43">
+        <v>200</v>
+      </c>
+      <c r="O43">
+        <v>221</v>
+      </c>
+      <c r="P43">
+        <v>221</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>3</v>
+      </c>
+      <c r="T43" t="s">
+        <v>118</v>
+      </c>
+      <c r="U43">
+        <v>4</v>
+      </c>
+      <c r="V43">
+        <v>44.6</v>
+      </c>
+      <c r="W43">
+        <v>30</v>
+      </c>
+      <c r="X43">
+        <v>25</v>
+      </c>
+      <c r="Y43" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>-63</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Carboxylate*")</f>
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*BSA*")</f>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Amine*")</f>
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Citrate*")</f>
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEG*")</f>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PEI*")</f>
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*PVP*")</f>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f>COUNTIF(Table1[[#This Row],[Ligands]],"*Au*")</f>
+        <v>0</v>
+      </c>
+      <c r="M44" t="s">
+        <v>56</v>
+      </c>
+      <c r="N44">
+        <v>200</v>
+      </c>
+      <c r="O44">
+        <v>221</v>
+      </c>
+      <c r="P44">
+        <v>221</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>3</v>
+      </c>
+      <c r="T44" t="s">
+        <v>118</v>
+      </c>
+      <c r="U44">
+        <v>4</v>
+      </c>
+      <c r="V44">
+        <v>4.46</v>
+      </c>
+      <c r="W44">
+        <v>30</v>
+      </c>
+      <c r="X44">
+        <v>25</v>
+      </c>
+      <c r="Y44" s="23" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>